<commit_message>
Push update on final report
</commit_message>
<xml_diff>
--- a/business_model.xlsx
+++ b/business_model.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanabsar/Documents/02_Education/01_ICL_BA/01_Modules/03_Summer Semester/01_AIB/AIB-Capstone-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FFE3B8C-0FC3-C74C-94EC-C1FBE30A2ED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A648DEB-A359-0E49-BC3D-AEADE8B6C202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" activeTab="2" xr2:uid="{F8864A3E-8F4B-7045-8E74-B4BB2A21AAC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
     <sheet name="COMPUTATION ==&gt;" sheetId="11" r:id="rId2"/>
-    <sheet name="curtailment" sheetId="10" r:id="rId3"/>
+    <sheet name="cashflow" sheetId="10" r:id="rId3"/>
     <sheet name="INPUT ==&gt;" sheetId="7" r:id="rId4"/>
     <sheet name="general_assumption" sheetId="8" r:id="rId5"/>
     <sheet name="BACK-UP ==&gt;" sheetId="6" r:id="rId6"/>
@@ -2308,12 +2308,13 @@
   <dimension ref="B1:X17513"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:24" x14ac:dyDescent="0.2">
@@ -2336,7 +2337,7 @@
     <row r="5" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C5" t="str">
         <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
-        <v>curtailment</v>
+        <v>cashflow</v>
       </c>
     </row>
     <row r="6" spans="2:24" x14ac:dyDescent="0.2">
@@ -54989,10 +54990,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE167E01-7078-E04D-B6A9-F6AFB67C52D3}">
-  <dimension ref="C1:J22"/>
+  <dimension ref="C1:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55203,6 +55204,46 @@
       <c r="H22" s="42"/>
       <c r="I22" s="42"/>
       <c r="J22" s="42"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="42"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="42"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C25" s="42"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C26" s="42"/>
+      <c r="D26" s="45"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
250524 - Update Business Model
</commit_message>
<xml_diff>
--- a/business_model.xlsx
+++ b/business_model.xlsx
@@ -8,22 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanabsar/Documents/02_Education/01_ICL_BA/01_Modules/03_Summer Semester/01_AIB/AIB-Capstone-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A648DEB-A359-0E49-BC3D-AEADE8B6C202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95B7945-AF62-2344-AE11-61768DABFA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19200" activeTab="2" xr2:uid="{F8864A3E-8F4B-7045-8E74-B4BB2A21AAC6}"/>
+    <workbookView xWindow="6940" yWindow="500" windowWidth="16800" windowHeight="19200" activeTab="3" xr2:uid="{F8864A3E-8F4B-7045-8E74-B4BB2A21AAC6}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="3" r:id="rId1"/>
     <sheet name="COMPUTATION ==&gt;" sheetId="11" r:id="rId2"/>
     <sheet name="cashflow" sheetId="10" r:id="rId3"/>
-    <sheet name="INPUT ==&gt;" sheetId="7" r:id="rId4"/>
-    <sheet name="general_assumption" sheetId="8" r:id="rId5"/>
-    <sheet name="BACK-UP ==&gt;" sheetId="6" r:id="rId6"/>
-    <sheet name="cost_model" sheetId="12" r:id="rId7"/>
-    <sheet name="TEMPLATE" sheetId="1" r:id="rId8"/>
+    <sheet name="energy_bill" sheetId="14" r:id="rId4"/>
+    <sheet name="customer_segment" sheetId="15" r:id="rId5"/>
+    <sheet name="INPUT ==&gt;" sheetId="7" r:id="rId6"/>
+    <sheet name="general_assumption" sheetId="8" r:id="rId7"/>
+    <sheet name="BACK-UP ==&gt;" sheetId="6" r:id="rId8"/>
+    <sheet name="cost_model" sheetId="12" r:id="rId9"/>
+    <sheet name="TEMPLATE" sheetId="1" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="DGDA">[1]Intro!$C$2</definedName>
@@ -52,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="155">
   <si>
     <t>Heat Smart Orkney</t>
   </si>
@@ -132,25 +134,7 @@
     <t>Introductiory tab with basic information and table of content</t>
   </si>
   <si>
-    <t>Selection of scenario and Dashboard with aggregated results of selected scenario</t>
-  </si>
-  <si>
     <t xml:space="preserve"> --- Section divider ---</t>
-  </si>
-  <si>
-    <t>Key financial results of selected scenario, by Phase and Asset Class</t>
-  </si>
-  <si>
-    <t>Overview of Quantum, GFA, and Land take of selected scenario, by Phase and Asset Class</t>
-  </si>
-  <si>
-    <t>Detailed financial results of selected scenario, by Phase and Asset Class</t>
-  </si>
-  <si>
-    <t>Detailed financial results of selected scenario, by Entity and Asset Class</t>
-  </si>
-  <si>
-    <t>GBP</t>
   </si>
   <si>
     <t>Key Metric</t>
@@ -323,16 +307,232 @@
   <si>
     <t>Contigency Buffer</t>
   </si>
+  <si>
+    <t>Wind Energy Consumption</t>
+  </si>
+  <si>
+    <t>Oil Energy Consumption</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Total Energy Consumed Per Day</t>
+  </si>
+  <si>
+    <t>Electric Energy Consumption</t>
+  </si>
+  <si>
+    <t>Stored/Curtailed Energy Used per day</t>
+  </si>
+  <si>
+    <t>Price of Curtailed Energy</t>
+  </si>
+  <si>
+    <t>kWh/Day</t>
+  </si>
+  <si>
+    <t>Price of Oil</t>
+  </si>
+  <si>
+    <t>Price Normal Energy</t>
+  </si>
+  <si>
+    <t>Energy Bill</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Oil</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>After</t>
+  </si>
+  <si>
+    <t>Avg Bill</t>
+  </si>
+  <si>
+    <t>Curtailed Energy Used</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Storage Heater</t>
+  </si>
+  <si>
+    <t>Normal Electric Heater</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t># Heater sold</t>
+  </si>
+  <si>
+    <t># Device sold</t>
+  </si>
+  <si>
+    <t>Average # of heater / Household</t>
+  </si>
+  <si>
+    <t>Average Total Energy Consumed Per day</t>
+  </si>
+  <si>
+    <t>kWh/day</t>
+  </si>
+  <si>
+    <t>£/kWh</t>
+  </si>
+  <si>
+    <t>£/kwh</t>
+  </si>
+  <si>
+    <t>£/day</t>
+  </si>
+  <si>
+    <t>cashflow</t>
+  </si>
+  <si>
+    <t>energy_bill</t>
+  </si>
+  <si>
+    <t>INPUT ==&gt;</t>
+  </si>
+  <si>
+    <t>general_assumption</t>
+  </si>
+  <si>
+    <t>BACK-UP ==&gt;</t>
+  </si>
+  <si>
+    <t>£</t>
+  </si>
+  <si>
+    <t>Daily Oil Consumption</t>
+  </si>
+  <si>
+    <t>Baseline Electricity Energy Consumption</t>
+  </si>
+  <si>
+    <t>Storage heater</t>
+  </si>
+  <si>
+    <t>% of household</t>
+  </si>
+  <si>
+    <t>Electric heater</t>
+  </si>
+  <si>
+    <t>Oil heater</t>
+  </si>
+  <si>
+    <t>Electric Quantum Heater</t>
+  </si>
+  <si>
+    <t>Oil Heater</t>
+  </si>
+  <si>
+    <t>Electricity Price</t>
+  </si>
+  <si>
+    <t>£/kwh - Referenced from fuel poverty strategy</t>
+  </si>
+  <si>
+    <t>Oil Price equ of electricity</t>
+  </si>
+  <si>
+    <t>Liter to kWh Oil</t>
+  </si>
+  <si>
+    <t>kwh/liter - https://www.rix.co.uk/blog/post/heating-oil-usage-calculator-how-much-heating-oil-am-i-using-variant-1#:~:text=Firstly%2C%20we%20need%20identify%20how,kWh%20of%20energy%20per%20litre.</t>
+  </si>
+  <si>
+    <t>Oil price per litere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">oil price per kwh </t>
+  </si>
+  <si>
+    <t>pence/liter - https://www.ons.gov.uk/economy/inflationandpriceindices/timeseries/kj5u/mm23</t>
+  </si>
+  <si>
+    <t>pence/kwh</t>
+  </si>
+  <si>
+    <t>kwh - derived from orkney wide energy audit 2014</t>
+  </si>
+  <si>
+    <t>Average Annual Oil Usage per household for heat</t>
+  </si>
+  <si>
+    <t>kwh - Referenced from fuel poverty strategy</t>
+  </si>
+  <si>
+    <t>Average Annual elec Usage per household for heat assume 50% for heat</t>
+  </si>
+  <si>
+    <t>Kaluza 1 device with 1 heaters charging (KWh)</t>
+  </si>
+  <si>
+    <t>With kaluza cost/day</t>
+  </si>
+  <si>
+    <t>Previous cost/day</t>
+  </si>
+  <si>
+    <t>Previous cost/month</t>
+  </si>
+  <si>
+    <t>With kaluza cost/month</t>
+  </si>
+  <si>
+    <t>pence</t>
+  </si>
+  <si>
+    <t>Price kaluza $/kwh</t>
+  </si>
+  <si>
+    <t>Saving absloute $</t>
+  </si>
+  <si>
+    <t>Household Income</t>
+  </si>
+  <si>
+    <t>Current Energy</t>
+  </si>
+  <si>
+    <t>Heating Energy</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>Savings per kWh</t>
+  </si>
+  <si>
+    <t>Device fee per month</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[$-409]dd\ mmm\ yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yy\ h\.mm;@"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="174" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -521,8 +721,44 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF156082"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F4E78"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -564,8 +800,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -679,16 +933,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color indexed="64"/>
+      </left>
+      <right style="dotted">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="41" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="25" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -806,12 +1088,84 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="28" fillId="7" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="27" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="41" fontId="28" fillId="7" borderId="0" xfId="4" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Calculation 2" xfId="3" xr:uid="{6EC7F68F-1F91-534E-AA89-56AA38990283}"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Input 2" xfId="2" xr:uid="{445D006A-BB22-8A4E-AC26-A3BB19736FAA}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Per cent" xfId="5" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -937,6 +1291,104 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B767BFE-3BF7-944F-9A81-62C89D0FBC7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="0"/>
+          <a:ext cx="1219200" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>584200</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E02D31C-B5C3-C946-A704-5812834D66B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="0"/>
+          <a:ext cx="1219200" cy="1219200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -981,7 +1433,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1030,7 +1482,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1557,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD64A031-B9CD-4F40-BE7E-476380549EFA}">
   <dimension ref="A1:AB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView showGridLines="0" topLeftCell="A18" zoomScale="200" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,7 +2192,7 @@
         <v>14</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>32</v>
+        <v>118</v>
       </c>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -2095,7 +2547,7 @@
         <v>1</v>
       </c>
       <c r="B30" s="47" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C30" s="24"/>
       <c r="D30" s="24"/>
@@ -2119,7 +2571,7 @@
         <v>2</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C31" s="24"/>
       <c r="D31" s="24"/>
@@ -2128,7 +2580,7 @@
         <v>Go To Sheet</v>
       </c>
       <c r="F31" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="O31" s="26"/>
       <c r="Q31" s="27" t="s">
@@ -2142,15 +2594,14 @@
         <f t="shared" ref="A32:A37" si="1">A31+1</f>
         <v>3</v>
       </c>
-      <c r="B32" s="41"/>
+      <c r="B32" s="41" t="s">
+        <v>113</v>
+      </c>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>26</v>
+        <v>Go To Sheet</v>
       </c>
       <c r="O32" s="26"/>
       <c r="Q32" s="27" t="s">
@@ -2164,16 +2615,16 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="B33" s="41"/>
+      <c r="B33" s="41" t="s">
+        <v>114</v>
+      </c>
       <c r="C33"/>
       <c r="D33"/>
       <c r="E33" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Go To Sheet</v>
       </c>
-      <c r="F33" s="28" t="s">
-        <v>27</v>
-      </c>
+      <c r="F33" s="28"/>
       <c r="O33" s="26"/>
       <c r="Q33" s="27" t="s">
         <v>2</v>
@@ -2186,15 +2637,17 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="B34" s="41"/>
+      <c r="B34" s="41" t="s">
+        <v>115</v>
+      </c>
       <c r="C34"/>
       <c r="D34"/>
       <c r="E34" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Go To Sheet</v>
       </c>
-      <c r="F34" s="9" t="s">
-        <v>28</v>
+      <c r="F34" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="O34" s="26"/>
       <c r="Q34" s="27" t="s">
@@ -2208,15 +2661,14 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="B35" s="41"/>
+      <c r="B35" s="41" t="s">
+        <v>116</v>
+      </c>
       <c r="C35"/>
       <c r="D35"/>
       <c r="E35" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>29</v>
+        <v>Go To Sheet</v>
       </c>
       <c r="O35" s="26"/>
       <c r="Q35" s="29" t="s">
@@ -2240,15 +2692,17 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="B36" s="41"/>
+      <c r="B36" s="41" t="s">
+        <v>117</v>
+      </c>
       <c r="C36"/>
       <c r="D36"/>
       <c r="E36" s="25" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Go To Sheet</v>
       </c>
-      <c r="F36" s="9" t="s">
-        <v>30</v>
+      <c r="F36" s="28" t="s">
+        <v>26</v>
       </c>
       <c r="O36" s="26"/>
     </row>
@@ -2264,11 +2718,54 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F37" s="9" t="s">
-        <v>31</v>
+      <c r="O37" s="26"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BEE0FD-5E8E-EA4F-A82C-2059E677659A}">
+  <dimension ref="C1:G7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E1" s="1"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="str">
+        <f>proj</f>
+        <v>Heat Smart Orkney</v>
       </c>
-      <c r="O37" s="26"/>
-    </row>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="3:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="str">
+        <f>sub_proj</f>
+        <v>Business Case</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
+        <v>TEMPLATE</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="str">
+        <f>HYPERLINK("#'Intro'!A1","Get Back to Table of Content")</f>
+        <v>Get Back to Table of Content</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2307,8 +2804,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9C1899B-0C34-9D4A-8278-A8062E785109}">
   <dimension ref="B1:X17513"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2440,13 +2937,13 @@
     </row>
     <row r="11" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B11" s="52" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C11" s="37"/>
     </row>
     <row r="12" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C12" s="51" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:24" x14ac:dyDescent="0.2">
@@ -54959,6 +55456,974 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B01D76-0DAC-CD45-826B-1079011915C2}">
+  <dimension ref="C1:J43"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C7" zoomScale="140" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection activeCell="C9" sqref="C9"/>
+      <selection pane="topRight" activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="44.6640625" customWidth="1"/>
+    <col min="5" max="10" width="25.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E1" s="1"/>
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="str">
+        <f>proj</f>
+        <v>Heat Smart Orkney</v>
+      </c>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="3:10" ht="19" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="str">
+        <f>sub_proj</f>
+        <v>Business Case</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
+        <v>energy_bill</v>
+      </c>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="str">
+        <f>HYPERLINK("#'Intro'!A1","Get Back to Table of Content")</f>
+        <v>Get Back to Table of Content</v>
+      </c>
+    </row>
+    <row r="7" spans="3:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="E9" s="63" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="63"/>
+      <c r="G9" s="65" t="s">
+        <v>103</v>
+      </c>
+      <c r="H9" s="65"/>
+      <c r="I9" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" s="64"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="D10" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="70">
+        <f>E14+E15</f>
+        <v>5.63</v>
+      </c>
+      <c r="F11" s="71">
+        <f>F14+F15</f>
+        <v>21.353287671232877</v>
+      </c>
+      <c r="G11" s="71">
+        <f>G14+G15</f>
+        <v>21.9</v>
+      </c>
+      <c r="H11" s="71">
+        <f>H14+H15</f>
+        <v>26.4</v>
+      </c>
+      <c r="I11" s="71">
+        <f>I14+I15</f>
+        <v>21.9</v>
+      </c>
+      <c r="J11" s="71">
+        <f>J14+J15</f>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="72">
+        <f>customer_segment!C37</f>
+        <v>11.223287671232876</v>
+      </c>
+      <c r="F12" s="73">
+        <f>E13-E13/$D$35*D33</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="73">
+        <v>0</v>
+      </c>
+      <c r="H12" s="73">
+        <v>0</v>
+      </c>
+      <c r="I12" s="73">
+        <v>0</v>
+      </c>
+      <c r="J12" s="73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="59" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="61" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="74">
+        <f>E12+E11</f>
+        <v>16.853287671232877</v>
+      </c>
+      <c r="F13" s="74">
+        <f>F11+F12</f>
+        <v>21.353287671232877</v>
+      </c>
+      <c r="G13" s="74">
+        <f>G11+G12</f>
+        <v>21.9</v>
+      </c>
+      <c r="H13" s="74">
+        <f>H11+H12</f>
+        <v>26.4</v>
+      </c>
+      <c r="I13" s="74">
+        <f>I11+I12</f>
+        <v>21.9</v>
+      </c>
+      <c r="J13" s="74">
+        <f>J11+J12</f>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D14" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" s="72">
+        <v>5.63</v>
+      </c>
+      <c r="F14" s="75">
+        <f>E13-F12-2.5*$D$34</f>
+        <v>14.353287671232877</v>
+      </c>
+      <c r="G14" s="72">
+        <v>21.9</v>
+      </c>
+      <c r="H14" s="75">
+        <f>G13-H12-2.5*$D$34</f>
+        <v>19.399999999999999</v>
+      </c>
+      <c r="I14" s="72">
+        <v>21.9</v>
+      </c>
+      <c r="J14" s="75">
+        <f>I13-J12-2.5*$D$34</f>
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>89</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="75">
+        <v>0</v>
+      </c>
+      <c r="F15" s="75">
+        <f>7*$D$34</f>
+        <v>7</v>
+      </c>
+      <c r="G15" s="75">
+        <v>0</v>
+      </c>
+      <c r="H15" s="75">
+        <f>7*$D$34</f>
+        <v>7</v>
+      </c>
+      <c r="I15" s="75">
+        <v>0</v>
+      </c>
+      <c r="J15" s="75">
+        <f>7*$D$34</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E16" s="72">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F16" s="72">
+        <f>$E$16</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G16" s="72">
+        <f t="shared" ref="G16:J16" si="0">$E$16</f>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H16" s="72">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I16" s="72">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="J16" s="72">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="60" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" s="72">
+        <v>0.22650045903448901</v>
+      </c>
+      <c r="F17" s="72">
+        <f>$E$17</f>
+        <v>0.22650045903448901</v>
+      </c>
+      <c r="G17" s="72">
+        <f t="shared" ref="G17:J17" si="1">$E$17</f>
+        <v>0.22650045903448901</v>
+      </c>
+      <c r="H17" s="72">
+        <f t="shared" si="1"/>
+        <v>0.22650045903448901</v>
+      </c>
+      <c r="I17" s="72">
+        <f t="shared" si="1"/>
+        <v>0.22650045903448901</v>
+      </c>
+      <c r="J17" s="72">
+        <f t="shared" si="1"/>
+        <v>0.22650045903448901</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="60" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="72">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="72">
+        <f>$E$18</f>
+        <v>0.15</v>
+      </c>
+      <c r="G18" s="72">
+        <f t="shared" ref="G18:J18" si="2">$E$18</f>
+        <v>0.15</v>
+      </c>
+      <c r="H18" s="72">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="I18" s="72">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+      <c r="J18" s="72">
+        <f t="shared" si="2"/>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C19" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E19" s="68">
+        <f>SUM(E11*E18,E12*E17,E15*E16)</f>
+        <v>3.3865798094103678</v>
+      </c>
+      <c r="F19" s="68">
+        <f>SUM(F14*F18,F12*F17,F15*F16)</f>
+        <v>2.6779931506849315</v>
+      </c>
+      <c r="G19" s="68">
+        <f>SUM(G14*G18,G12*G17,G15*G16)</f>
+        <v>3.2849999999999997</v>
+      </c>
+      <c r="H19" s="68">
+        <f>SUM(H14*H18,H12*H17,H15*H16)</f>
+        <v>3.4349999999999996</v>
+      </c>
+      <c r="I19" s="68">
+        <f>SUM(I14*I18,I12*I17,I15*I16)</f>
+        <v>3.2849999999999997</v>
+      </c>
+      <c r="J19" s="68">
+        <f>SUM(J14*J18,J12*J17,J15*J16)</f>
+        <v>3.4349999999999996</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="D20" s="61" t="s">
+        <v>111</v>
+      </c>
+      <c r="E20" s="68">
+        <f>E19/E13</f>
+        <v>0.20094475781072499</v>
+      </c>
+      <c r="F20" s="68">
+        <f>F19/F13</f>
+        <v>0.1254136221043245</v>
+      </c>
+      <c r="G20" s="68">
+        <f>G19/G13</f>
+        <v>0.15</v>
+      </c>
+      <c r="H20" s="68">
+        <f>H19/H13</f>
+        <v>0.13011363636363635</v>
+      </c>
+      <c r="I20" s="68">
+        <f>I19/I13</f>
+        <v>0.15</v>
+      </c>
+      <c r="J20" s="68">
+        <f>J19/J13</f>
+        <v>0.13011363636363635</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="62" t="s">
+        <v>101</v>
+      </c>
+      <c r="E21" s="60">
+        <f>E15/E13</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="67">
+        <f>F15/F13</f>
+        <v>0.32781837194233987</v>
+      </c>
+      <c r="G21" s="67">
+        <f>G15/G13</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="67">
+        <f>H15/H13</f>
+        <v>0.26515151515151514</v>
+      </c>
+      <c r="I21" s="67">
+        <f>I15/I13</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="67">
+        <f>J15/J13</f>
+        <v>0.26515151515151514</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="55" t="s">
+        <v>151</v>
+      </c>
+      <c r="D22" s="62"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="59" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="69">
+        <f>E19*30</f>
+        <v>101.59739428231103</v>
+      </c>
+      <c r="F23" s="69">
+        <f t="shared" ref="F23:J23" si="3">F19*30</f>
+        <v>80.33979452054794</v>
+      </c>
+      <c r="G23" s="69">
+        <f t="shared" si="3"/>
+        <v>98.55</v>
+      </c>
+      <c r="H23" s="69">
+        <f t="shared" si="3"/>
+        <v>103.04999999999998</v>
+      </c>
+      <c r="I23" s="69">
+        <f t="shared" si="3"/>
+        <v>98.55</v>
+      </c>
+      <c r="J23" s="69">
+        <f t="shared" si="3"/>
+        <v>103.04999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D24" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="E24" s="81">
+        <f>IF(E10&lt;&gt;"Before",(D20-E20)/D20,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="81">
+        <f t="shared" ref="F24:J24" si="4">IF(F10&lt;&gt;"Before",(E20-F20)/E20,0)</f>
+        <v>0.37588010022906498</v>
+      </c>
+      <c r="G24" s="81">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="81">
+        <f t="shared" si="4"/>
+        <v>0.13257575757575765</v>
+      </c>
+      <c r="I24" s="81">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="81">
+        <f t="shared" si="4"/>
+        <v>0.13257575757575765</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C25" s="59" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="E25" s="82">
+        <f>IF(E$10&lt;&gt;"Before",D23-E23,0)</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="82">
+        <f>IF(F$10&lt;&gt;"Before",E23-F23,0)</f>
+        <v>21.257599761763089</v>
+      </c>
+      <c r="G25" s="82">
+        <f t="shared" ref="F25:J25" si="5">IF(G$10&lt;&gt;"Before",F23-G23,0)</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="82">
+        <f>IF(H$10&lt;&gt;"Before",G23-H23,0)</f>
+        <v>-4.4999999999999858</v>
+      </c>
+      <c r="I25" s="82">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="82">
+        <f t="shared" si="5"/>
+        <v>-4.4999999999999858</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C26" s="59" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="61"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="61"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C27" s="59" t="s">
+        <v>154</v>
+      </c>
+      <c r="D27" s="61"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="61"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="F31" s="69">
+        <f>E23-F23</f>
+        <v>21.257599761763089</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C32" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33">
+        <f>D34</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>107</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36">
+        <v>21.9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D38">
+        <v>16.27</v>
+      </c>
+      <c r="E38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>120</v>
+      </c>
+      <c r="D39">
+        <v>5.63</v>
+      </c>
+      <c r="E39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+      <c r="D41" s="56">
+        <v>0.1</v>
+      </c>
+      <c r="E41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>123</v>
+      </c>
+      <c r="D42" s="56">
+        <v>0.31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D43" s="56">
+        <v>0.36</v>
+      </c>
+      <c r="E43" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="I16:J18" unlockedFormula="1"/>
+  </ignoredErrors>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C12669-A427-0E42-BD18-786A908F526B}">
+  <dimension ref="C1:G37"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="C22" zoomScale="180" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="71.33203125" customWidth="1"/>
+    <col min="4" max="6" width="24.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="E1" s="1"/>
+      <c r="G1" s="2"/>
+    </row>
+    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C2" s="1" t="str">
+        <f>proj</f>
+        <v>Heat Smart Orkney</v>
+      </c>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="3:7" ht="19" x14ac:dyDescent="0.2">
+      <c r="C3" s="3" t="str">
+        <f>sub_proj</f>
+        <v>Business Case</v>
+      </c>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C5" t="str">
+        <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
+        <v>customer_segment</v>
+      </c>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="str">
+        <f>HYPERLINK("#'Intro'!A1","Get Back to Table of Content")</f>
+        <v>Get Back to Table of Content</v>
+      </c>
+    </row>
+    <row r="7" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C9" s="58" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="E9" s="58" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C10" s="77" t="s">
+        <v>142</v>
+      </c>
+      <c r="D10" s="79">
+        <f>D33*D32</f>
+        <v>1.5873152169136961</v>
+      </c>
+      <c r="E10" s="79">
+        <f>D33*D26</f>
+        <v>1.0939487999999999</v>
+      </c>
+      <c r="F10" s="79">
+        <f>D33*D26</f>
+        <v>1.0939487999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C11" s="77" t="s">
+        <v>141</v>
+      </c>
+      <c r="D11" s="79">
+        <f>D33*D34</f>
+        <v>0.52559999999999996</v>
+      </c>
+      <c r="E11" s="79">
+        <f>D33*D34</f>
+        <v>0.52559999999999996</v>
+      </c>
+      <c r="F11" s="79">
+        <f>D33*D34</f>
+        <v>0.52559999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C12" s="77" t="s">
+        <v>143</v>
+      </c>
+      <c r="D12" s="79">
+        <f>D10*30</f>
+        <v>47.619456507410888</v>
+      </c>
+      <c r="E12" s="79">
+        <f>E10*30</f>
+        <v>32.818463999999999</v>
+      </c>
+      <c r="F12" s="79">
+        <f>F10*30</f>
+        <v>32.818463999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C13" s="77" t="s">
+        <v>144</v>
+      </c>
+      <c r="D13" s="79">
+        <f>D11*30</f>
+        <v>15.767999999999999</v>
+      </c>
+      <c r="E13" s="79">
+        <f t="shared" ref="E13:F13" si="0">E11*30</f>
+        <v>15.767999999999999</v>
+      </c>
+      <c r="F13" s="79">
+        <f t="shared" si="0"/>
+        <v>15.767999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C14" s="77" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="79">
+        <f>D12-D13</f>
+        <v>31.851456507410887</v>
+      </c>
+      <c r="E14" s="79">
+        <f>E12-E13</f>
+        <v>17.050463999999998</v>
+      </c>
+      <c r="F14" s="79">
+        <f t="shared" ref="E14:F14" si="1">F12-F13</f>
+        <v>17.050463999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="78">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18">
+        <v>21.88</v>
+      </c>
+      <c r="E18">
+        <f>D18*0.15*365</f>
+        <v>1197.9299999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D19">
+        <v>7.008</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <f>(D18+D19)*0.15*365</f>
+        <v>1581.6179999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C25" s="58" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="58" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="75">
+        <v>0.15609999999999999</v>
+      </c>
+      <c r="E26" s="76" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="75">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>130</v>
+      </c>
+      <c r="D28" s="75">
+        <v>10.35</v>
+      </c>
+      <c r="E28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D29" s="75">
+        <f>D27/D28</f>
+        <v>4.3478260869565215</v>
+      </c>
+      <c r="E29" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="75">
+        <v>21340.76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D31" s="75">
+        <f>8193*0.5</f>
+        <v>4096.5</v>
+      </c>
+      <c r="E31" s="76" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>129</v>
+      </c>
+      <c r="D32" s="75">
+        <f>(D30/D31*D29)/100</f>
+        <v>0.22650045903448859</v>
+      </c>
+      <c r="E32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="75">
+        <v>7.008</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D34" s="75">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="66">
+        <f>(D32-D26)/D32</f>
+        <v>0.31081817376700732</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C37" s="80">
+        <f>D31/365</f>
+        <v>11.223287671232876</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52E197F1-72C8-A04F-A3CC-3B3D594A0156}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -54988,12 +56453,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE167E01-7078-E04D-B6A9-F6AFB67C52D3}">
   <dimension ref="C1:J26"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="J38" sqref="H38:J41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55039,13 +56504,13 @@
     <row r="7" spans="3:10" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C11" s="48" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F11" s="48"/>
       <c r="G11" s="48"/>
@@ -55055,7 +56520,7 @@
     </row>
     <row r="12" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C12" s="42" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D12" s="45">
         <v>2017</v>
@@ -55079,7 +56544,7 @@
     </row>
     <row r="14" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C14" s="42" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D14" s="46">
         <v>0.05</v>
@@ -55103,13 +56568,13 @@
     </row>
     <row r="16" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C16" s="42" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D16" s="45">
         <v>100</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
@@ -55119,13 +56584,13 @@
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C17" s="42" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D17" s="45">
         <v>80</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F17" s="42"/>
       <c r="G17" s="42"/>
@@ -55135,13 +56600,13 @@
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C18" s="42" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D18" s="45">
         <v>100</v>
       </c>
       <c r="E18" s="43" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F18" s="42"/>
       <c r="G18" s="42"/>
@@ -55151,7 +56616,7 @@
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C19" s="42" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D19" s="45">
         <v>0.1</v>
@@ -55175,13 +56640,13 @@
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C21" s="42" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D21" s="45">
         <v>1.2</v>
       </c>
       <c r="E21" s="43" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F21" s="42"/>
       <c r="G21" s="42"/>
@@ -55191,13 +56656,13 @@
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.2">
       <c r="C22" s="42" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D22" s="45">
         <v>10</v>
       </c>
       <c r="E22" s="43" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F22" s="42"/>
       <c r="G22" s="42"/>
@@ -55251,7 +56716,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6680F34B-135D-9045-A897-BEB4736AC73A}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -55281,7 +56746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C66CD16-DDDC-6A44-B460-9C435814ECD4}">
   <dimension ref="C1:I94"/>
   <sheetViews>
@@ -55327,40 +56792,40 @@
     <row r="7" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D11">
         <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D12">
         <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D17">
         <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D18" s="56">
         <v>0.1</v>
@@ -55368,90 +56833,90 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D20">
         <v>1.2</v>
       </c>
       <c r="E20" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D21">
         <v>10</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D53" s="55" t="s">
+        <v>35</v>
+      </c>
+      <c r="E53" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="G53" s="52" t="s">
+        <v>49</v>
+      </c>
+      <c r="H53" t="s">
+        <v>50</v>
+      </c>
+      <c r="I53" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C54" s="52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="55" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D55" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="E55" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D56" t="s">
+        <v>39</v>
+      </c>
+      <c r="E56" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>40</v>
+      </c>
+      <c r="E57" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="58" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D59" t="s">
         <v>41</v>
       </c>
-      <c r="E53" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="G53" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="H53" t="s">
-        <v>56</v>
-      </c>
-      <c r="I53" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="54" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C54" s="52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D55" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="E55" s="54" t="s">
+    </row>
+    <row r="60" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D60" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D56" t="s">
-        <v>45</v>
-      </c>
-      <c r="E56" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="57" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D57" t="s">
-        <v>46</v>
-      </c>
-      <c r="E57" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="58" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D58" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="59" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D59" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="60" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D60" t="s">
-        <v>60</v>
-      </c>
-    </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G62">
         <v>100</v>
@@ -55459,48 +56924,48 @@
     </row>
     <row r="64" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C64" s="52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D65" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="E65" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D66" t="s">
+        <v>38</v>
+      </c>
+      <c r="E66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D67" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D68" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D70" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C71" s="52" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D65" s="54" t="s">
-        <v>53</v>
-      </c>
-      <c r="E65" s="54" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D66" t="s">
-        <v>44</v>
-      </c>
-      <c r="E66" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D67" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D68" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="D70" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C71" s="52" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D72" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G72">
         <f>689/2</f>
@@ -55517,12 +56982,12 @@
     </row>
     <row r="74" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D74" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D78">
         <v>1000</v>
@@ -55530,7 +56995,7 @@
     </row>
     <row r="79" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D79">
         <v>50</v>
@@ -55538,39 +57003,39 @@
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D80">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D81">
         <v>2</v>
       </c>
       <c r="E81" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C86" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D86">
         <f>SUM(D78:D79)</f>
@@ -55579,100 +57044,54 @@
     </row>
     <row r="88" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C88" s="52" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D88" s="52" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E88" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C89" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D89">
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C90" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E90" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C91" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="92" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C92" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C93" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="94" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C94" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4BEE0FD-5E8E-EA4F-A82C-2059E677659A}">
-  <dimension ref="C1:G7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="E1" s="1"/>
-      <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="1" t="str">
-        <f>proj</f>
-        <v>Heat Smart Orkney</v>
-      </c>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="3:7" ht="19" x14ac:dyDescent="0.2">
-      <c r="C3" s="3" t="str">
-        <f>sub_proj</f>
-        <v>Business Case</v>
-      </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C5" t="str">
-        <f ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
-        <v>TEMPLATE</v>
-      </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.2">
-      <c r="C6" s="4" t="str">
-        <f>HYPERLINK("#'Intro'!A1","Get Back to Table of Content")</f>
-        <v>Get Back to Table of Content</v>
-      </c>
-    </row>
-    <row r="7" spans="3:7" s="5" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>